<commit_message>
change opcode of some instructions
</commit_message>
<xml_diff>
--- a/HALFMIPS.xlsx
+++ b/HALFMIPS.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MARO\work\github\BINUTILS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF7235D-BE17-420C-9567-6942C52ADA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIPS-I" sheetId="4" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="137">
   <si>
     <t>bits 28..26</t>
   </si>
@@ -421,12 +427,18 @@
   </si>
   <si>
     <t>HDIVU</t>
+  </si>
+  <si>
+    <t>LWC0</t>
+  </si>
+  <si>
+    <t>SWC0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -479,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -506,6 +518,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -520,6 +535,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -895,7 +913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -906,16 +924,16 @@
       <c r="A1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
@@ -974,7 +992,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
@@ -983,10 +1001,10 @@
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1009,7 +1027,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1042,7 +1060,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1075,7 +1093,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1108,7 +1126,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1141,7 +1159,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1174,15 +1192,15 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="1">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
+      <c r="D10" s="11" t="s">
+        <v>135</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>44</v>
@@ -1207,15 +1225,15 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="1">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
+      <c r="D11" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>47</v>
@@ -1246,16 +1264,16 @@
       <c r="B14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
@@ -1314,7 +1332,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="1">
@@ -1349,7 +1367,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="1">
         <v>1</v>
       </c>
@@ -1382,7 +1400,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -1415,7 +1433,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -1448,7 +1466,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -1481,7 +1499,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="1">
         <v>5</v>
       </c>
@@ -1514,7 +1532,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -1547,7 +1565,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="1">
         <v>7</v>
       </c>
@@ -1586,16 +1604,16 @@
       <c r="B27" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
@@ -1654,7 +1672,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>86</v>
       </c>
       <c r="B30" s="1">
@@ -1689,7 +1707,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="1">
         <v>1</v>
       </c>
@@ -1722,7 +1740,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="1">
         <v>2</v>
       </c>
@@ -1755,7 +1773,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="1">
         <v>3</v>
       </c>
@@ -1994,7 +2012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -2005,16 +2023,16 @@
       <c r="A1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
@@ -2073,7 +2091,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
@@ -2108,7 +2126,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -2141,7 +2159,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -2174,7 +2192,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -2207,7 +2225,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -2240,7 +2258,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -2273,15 +2291,15 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="1">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>116</v>
+      <c r="D10" s="11" t="s">
+        <v>135</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>44</v>
@@ -2293,28 +2311,28 @@
         <v>46</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="J10" s="10" t="s">
-        <v>31</v>
+      <c r="J10" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="1">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
+      <c r="D11" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>47</v>
@@ -2345,16 +2363,16 @@
       <c r="B14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
@@ -2413,7 +2431,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="1">
@@ -2448,7 +2466,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="1">
         <v>1</v>
       </c>
@@ -2481,7 +2499,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -2514,7 +2532,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -2547,7 +2565,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -2580,7 +2598,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="1">
         <v>5</v>
       </c>
@@ -2605,15 +2623,15 @@
       <c r="I22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>31</v>
+      <c r="J22" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -2646,7 +2664,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="1">
         <v>7</v>
       </c>
@@ -2656,20 +2674,20 @@
       <c r="D24" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="G24" s="7" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="I24" s="7" t="s">
         <v>126</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>127</v>
@@ -2685,16 +2703,16 @@
       <c r="B27" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
@@ -2753,7 +2771,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>86</v>
       </c>
       <c r="B30" s="1">
@@ -2788,7 +2806,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="1">
         <v>1</v>
       </c>
@@ -2821,7 +2839,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="1">
         <v>2</v>
       </c>
@@ -2854,7 +2872,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="1">
         <v>3</v>
       </c>
@@ -3093,7 +3111,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3101,5 +3119,6 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>